<commit_message>
Forced push - to gauge CR update
</commit_message>
<xml_diff>
--- a/reqs/testAccts.xlsx
+++ b/reqs/testAccts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects_sdk\cb\compass\reqs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects_sdk\cb\compass-auto-poc\reqs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95D6A75-69DD-4A16-84CB-0757CEC495D6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Accounts" sheetId="1" r:id="rId1"/>
@@ -29,9 +30,6 @@
     <definedName name="Vendor">#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
-  <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-  </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="142">
   <si>
     <t>Test Group</t>
   </si>
@@ -468,21 +466,12 @@
   </si>
   <si>
     <t>carrie.reid@cbrands.com</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Count of Business Role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -670,7 +659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -710,11 +699,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -838,654 +822,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Vik Sharma" refreshedDate="42975.937238078703" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="31">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L32" sheet="Test Accounts"/>
-  </cacheSource>
-  <cacheFields count="12">
-    <cacheField name="Test Group" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Business Role" numFmtId="0">
-      <sharedItems count="22">
-        <s v="GEO BU COORDINATOR"/>
-        <s v="GEO BU OPS DIRECTOR"/>
-        <s v="GEO BU VP"/>
-        <s v="GEO BUAM"/>
-        <s v="GM"/>
-        <s v="MDM"/>
-        <s v="Non-Sales"/>
-        <s v="OFF BU VP"/>
-        <s v="OFF CHANNEL VP"/>
-        <s v="OFF KAM"/>
-        <s v="OFF NAM"/>
-        <s v="OFF NAM ROLL-UP"/>
-        <s v="OFF PREM CHAIN/INDEP SPEC"/>
-        <s v="ON BU VP"/>
-        <s v="ON KAM"/>
-        <s v="ON NAM"/>
-        <s v="ON PREM ACT MGR"/>
-        <s v="ON PREM ACT SPEC"/>
-        <s v="ON PREM DEV MGR"/>
-        <s v="ON PREM DIRECTOR"/>
-        <s v="ON PREM MGR"/>
-        <s v="REGIONAL CHAIN DIRECTOR"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Sales Collab XRef Role" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Business Unit" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="OIM Test Account Reason Desc" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="OIM Roles" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Name" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Person ID" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Employee ID" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="User ID" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Pswd:" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Notes" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="31">
-  <r>
-    <s v="Tester 4 &amp; Tester 5"/>
-    <x v="0"/>
-    <s v="BU"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-SALESCOORDINATOR"/>
-    <s v="Katrina Olson"/>
-    <m/>
-    <m/>
-    <s v="katrina.olson@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Non Data Science Market + BU Administrative/Analytical Roles"/>
-  </r>
-  <r>
-    <s v="Tester 4 &amp; Tester 5"/>
-    <x v="1"/>
-    <s v="BU"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-BUSUNITOPRMGR"/>
-    <s v="Julie Graham"/>
-    <m/>
-    <m/>
-    <s v="julie.graham@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Non Data Science Market + BU Administrative/Analytical Roles"/>
-  </r>
-  <r>
-    <s v="Tester 1"/>
-    <x v="2"/>
-    <s v="BU"/>
-    <s v="East Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-BUSUNITVP"/>
-    <s v="Jim O'Neil"/>
-    <m/>
-    <m/>
-    <s v="jim.oneil@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Manhattan specific GSM Use Cases + Data Science Market"/>
-  </r>
-  <r>
-    <s v="Tester 2"/>
-    <x v="2"/>
-    <s v="BU"/>
-    <s v="West Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-BUSUNITVP"/>
-    <s v="Stash Rowley"/>
-    <m/>
-    <m/>
-    <s v="stash.rowley@devcbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Data Science Market"/>
-  </r>
-  <r>
-    <s v="Tester 3"/>
-    <x v="2"/>
-    <s v="BU"/>
-    <s v="Southeast Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-BUSUNITVP"/>
-    <s v="Lisa Scalise-Boswell"/>
-    <m/>
-    <m/>
-    <s v="lisa.scalise-boswell@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Non Data Science Market"/>
-  </r>
-  <r>
-    <s v="Tester 4 &amp; Tester 5"/>
-    <x v="2"/>
-    <s v="BU"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-BUSUNITVP"/>
-    <s v="John Utter"/>
-    <m/>
-    <m/>
-    <s v="john.utter@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Regional Off &amp; On Prem Chain role testing"/>
-  </r>
-  <r>
-    <s v="Tester 4 &amp; Tester 5"/>
-    <x v="3"/>
-    <s v="BU"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-BUSUNITANALYST"/>
-    <s v="Mark Bortscheller"/>
-    <m/>
-    <m/>
-    <s v="mark.bortscheller@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Non Data Science Market + BU Administrative/Analytical Roles"/>
-  </r>
-  <r>
-    <s v="Tester 1"/>
-    <x v="4"/>
-    <s v="GM"/>
-    <s v="East Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-GENMGR"/>
-    <s v="Fred Berrios"/>
-    <m/>
-    <m/>
-    <s v="fred.berrios@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Manhattan specific GSM Use Cases + Data Science Market"/>
-  </r>
-  <r>
-    <s v="Tester 2"/>
-    <x v="4"/>
-    <s v="GM"/>
-    <s v="West Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-GENMGR"/>
-    <s v="Mark Nobles"/>
-    <m/>
-    <m/>
-    <s v="mark.nobles@devcbrands.com"/>
-    <s v="Corona.2016"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Tester 3"/>
-    <x v="4"/>
-    <s v="GM"/>
-    <s v="Southeast Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-GENMGR"/>
-    <s v="Joe Delapaz"/>
-    <m/>
-    <m/>
-    <s v="joe.delapaz@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Tester 4"/>
-    <x v="4"/>
-    <s v="GM"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-GENMGR"/>
-    <s v="Robert Van Witzenburg"/>
-    <m/>
-    <m/>
-    <s v="robert.vanwitzenburg@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Regional Off &amp; On Prem Chain role testing"/>
-  </r>
-  <r>
-    <s v="Tester 1"/>
-    <x v="5"/>
-    <s v="MDM"/>
-    <s v="East Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-MKTDEVMGR"/>
-    <s v="John Hoban"/>
-    <m/>
-    <m/>
-    <s v="john.hoban@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Manhattan specific GSM Use Cases + Data Science Market"/>
-  </r>
-  <r>
-    <s v="Tester 2"/>
-    <x v="5"/>
-    <s v="MDM"/>
-    <s v="West Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-MKTDEVMGR"/>
-    <s v="Juan Baez"/>
-    <m/>
-    <m/>
-    <s v="juan.baez@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Tester 3"/>
-    <x v="5"/>
-    <s v="MDM"/>
-    <s v="Southeast Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-MKTDEVMGR"/>
-    <s v="Chris Williams"/>
-    <m/>
-    <m/>
-    <s v="chris.williams@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Tester 4"/>
-    <x v="5"/>
-    <s v="MDM"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-BIZ-ROLE-MKTDEVMGR"/>
-    <s v="Carrie Reid"/>
-    <m/>
-    <m/>
-    <s v="carrie.reid@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Regional Off &amp; On Prem Chain role testing"/>
-  </r>
-  <r>
-    <s v="Tester 8"/>
-    <x v="6"/>
-    <s v="EXEC/CORPORATE VIEW"/>
-    <s v="Not Applicable"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Colleen McLaughlin"/>
-    <m/>
-    <m/>
-    <s v="colleen.mclaughlin@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Tester 7"/>
-    <x v="7"/>
-    <s v="BU"/>
-    <s v="Off Prem Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Pat O'Dea"/>
-    <m/>
-    <m/>
-    <s v="pat.odea@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 7"/>
-    <x v="8"/>
-    <s v="CHANNEL"/>
-    <s v="Off Prem Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Shawn Keller"/>
-    <m/>
-    <m/>
-    <s v="shawn.keller@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National Off Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="9"/>
-    <s v="KAM"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Blake Kohlbrecher"/>
-    <m/>
-    <m/>
-    <s v="blake.kohlbrecher@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Regional Off &amp; On Prem Chain role testing"/>
-  </r>
-  <r>
-    <s v="Tester 7"/>
-    <x v="10"/>
-    <s v="NAM"/>
-    <s v="Off Prem Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Eric Ramey"/>
-    <m/>
-    <m/>
-    <s v="eric.ramey@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National Off Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 7"/>
-    <x v="11"/>
-    <s v="TEAM"/>
-    <s v="Off Prem Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Brian Key"/>
-    <m/>
-    <m/>
-    <s v="brian.key@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National Off Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="12"/>
-    <s v="NEW - IN PROG"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Chelsea Hoff"/>
-    <m/>
-    <m/>
-    <s v="chelsea.hoff@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Regional Off &amp; On Prem Chain role testing"/>
-  </r>
-  <r>
-    <s v="Tester 6"/>
-    <x v="13"/>
-    <s v="GEOGRAPHIC"/>
-    <s v="On Prem Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Cathy Popick"/>
-    <m/>
-    <m/>
-    <s v="cathy.popick@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="14"/>
-    <s v="KAM"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Kelly Moorehead"/>
-    <m/>
-    <m/>
-    <s v="kelly.moorehead@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 6"/>
-    <x v="15"/>
-    <s v="NAM"/>
-    <s v="On Prem Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Fred Ashenbrenner"/>
-    <m/>
-    <m/>
-    <s v="fred.ashenbrenner@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="16"/>
-    <s v="AM"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Jamie Weiler"/>
-    <m/>
-    <m/>
-    <s v="jamie.weiler@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 8"/>
-    <x v="17"/>
-    <s v="AR"/>
-    <s v="Southwest Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Brittany Wilson"/>
-    <m/>
-    <m/>
-    <s v="brittany.wilson@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="18"/>
-    <s v="DM"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Andy Keefner"/>
-    <m/>
-    <m/>
-    <s v="andy.keefner@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 8"/>
-    <x v="19"/>
-    <s v="DIRECTOR"/>
-    <s v="Southeast Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Alex Prieto"/>
-    <m/>
-    <m/>
-    <s v="alex.prieto@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="20"/>
-    <s v="EXEC"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="George O'Hare"/>
-    <m/>
-    <m/>
-    <s v="george.ohare@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="National On Prem team roles + reporting relationship/rollups"/>
-  </r>
-  <r>
-    <s v="Tester 5"/>
-    <x v="21"/>
-    <s v="CHANNEL"/>
-    <s v="Central Business Unit"/>
-    <s v="Beer Field Sales Enablement Program Testing"/>
-    <s v="UG-CBIGDC-ROLE-EcrownAppUserCorporateView"/>
-    <s v="Bill Havle"/>
-    <m/>
-    <m/>
-    <s v="bill.havle@cbrands.com"/>
-    <s v="Corona.2016"/>
-    <s v="Regional Off &amp; On Prem Chain role testing"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B37:C60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" subtotalTop="0" showAll="0">
-      <items count="23">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="23">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Business Role" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1750,30 +1086,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" customWidth="1"/>
-    <col min="10" max="10" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +1147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
@@ -1835,7 +1171,7 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="37" t="s">
         <v>63</v>
       </c>
       <c r="K2" s="10" t="s">
@@ -1845,7 +1181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>46</v>
       </c>
@@ -1879,7 +1215,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1913,7 +1249,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>30</v>
       </c>
@@ -1947,7 +1283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>37</v>
       </c>
@@ -1981,7 +1317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>46</v>
       </c>
@@ -2015,7 +1351,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -2049,7 +1385,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
@@ -2083,7 +1419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>30</v>
       </c>
@@ -2115,7 +1451,7 @@
       </c>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>37</v>
       </c>
@@ -2147,7 +1483,7 @@
       </c>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
@@ -2181,7 +1517,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
@@ -2215,7 +1551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>30</v>
       </c>
@@ -2247,7 +1583,7 @@
       </c>
       <c r="L14" s="23"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>37</v>
       </c>
@@ -2279,7 +1615,7 @@
       </c>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>64</v>
       </c>
@@ -2313,7 +1649,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>87</v>
       </c>
@@ -2345,7 +1681,7 @@
       </c>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>118</v>
       </c>
@@ -2379,7 +1715,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>118</v>
       </c>
@@ -2413,7 +1749,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -2447,7 +1783,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>118</v>
       </c>
@@ -2481,7 +1817,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>118</v>
       </c>
@@ -2515,7 +1851,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>68</v>
       </c>
@@ -2549,7 +1885,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>108</v>
       </c>
@@ -2583,7 +1919,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>68</v>
       </c>
@@ -2617,7 +1953,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>108</v>
       </c>
@@ -2651,7 +1987,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>68</v>
       </c>
@@ -2685,7 +2021,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>87</v>
       </c>
@@ -2719,7 +2055,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>68</v>
       </c>
@@ -2753,7 +2089,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>87</v>
       </c>
@@ -2787,7 +2123,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>68</v>
       </c>
@@ -2821,7 +2157,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>68</v>
       </c>
@@ -2855,238 +2191,46 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="C37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="C46" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C59" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="C60" s="39">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L1">
+  <autoFilter ref="A1:L1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:L32">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="J17" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J9" r:id="rId4"/>
-    <hyperlink ref="J13" r:id="rId5"/>
-    <hyperlink ref="J14" r:id="rId6"/>
-    <hyperlink ref="J11" r:id="rId7"/>
-    <hyperlink ref="J15" r:id="rId8"/>
-    <hyperlink ref="J3" r:id="rId9"/>
-    <hyperlink ref="J2" r:id="rId10"/>
-    <hyperlink ref="J29" r:id="rId11"/>
-    <hyperlink ref="J30" r:id="rId12"/>
-    <hyperlink ref="J25" r:id="rId13"/>
-    <hyperlink ref="J27" r:id="rId14"/>
-    <hyperlink ref="J28" r:id="rId15"/>
-    <hyperlink ref="J31" r:id="rId16"/>
-    <hyperlink ref="J24" r:id="rId17"/>
-    <hyperlink ref="J26" r:id="rId18"/>
-    <hyperlink ref="J18" r:id="rId19"/>
-    <hyperlink ref="J19" r:id="rId20"/>
-    <hyperlink ref="J22" r:id="rId21"/>
-    <hyperlink ref="J21" r:id="rId22"/>
-    <hyperlink ref="J6" r:id="rId23"/>
-    <hyperlink ref="J7" r:id="rId24"/>
-    <hyperlink ref="J12" r:id="rId25"/>
-    <hyperlink ref="J23" r:id="rId26"/>
-    <hyperlink ref="J32" r:id="rId27"/>
-    <hyperlink ref="J20" r:id="rId28"/>
-    <hyperlink ref="J10" r:id="rId29" display="mailto:mark.nobles@devcbrands.com"/>
-    <hyperlink ref="J5" r:id="rId30" display="mailto:stash.rowley@devcbrands.com"/>
-    <hyperlink ref="J16" r:id="rId31"/>
-    <hyperlink ref="J8" r:id="rId32"/>
+    <hyperlink ref="J17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J2" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J29" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J30" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J25" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J27" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J28" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J31" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J26" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J18" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J6" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J12" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J23" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="J32" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J20" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="J10" r:id="rId28" display="mailto:mark.nobles@devcbrands.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="J5" r:id="rId29" display="mailto:stash.rowley@devcbrands.com" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="J16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="J8" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId33"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>